<commit_message>
model changes final submit
</commit_message>
<xml_diff>
--- a/projects/validation - single vehicle motion/docs/ips.xlsx
+++ b/projects/validation - single vehicle motion/docs/ips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\research\sae-2021\vehicle-dymanimcs-malibu\engineering\inertial-parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joe/Documents/pycrash/projects/validation - single vehicle motion/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C2756F-75E9-4B12-94F8-F625C7B9C461}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DD3F18-72EF-D641-A776-CEEA68CC8E5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9720" yWindow="2985" windowWidth="24270" windowHeight="17280" xr2:uid="{E0D980B0-3EDE-4883-8BEE-1B06EFC1FF71}"/>
+    <workbookView xWindow="4900" yWindow="3020" windowWidth="37460" windowHeight="20800" xr2:uid="{E0D980B0-3EDE-4883-8BEE-1B06EFC1FF71}"/>
   </bookViews>
   <sheets>
     <sheet name="For HVE" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'For HVE'!$A$1:$I$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'IPs From 2019 SAE Pub'!$A$1:$D$48</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -857,8 +860,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="0.0000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -1702,9 +1705,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1714,7 +1714,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1723,33 +1723,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1789,15 +1762,6 @@
     <xf numFmtId="164" fontId="9" fillId="4" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1815,15 +1779,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1852,19 +1807,10 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="33" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="33" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1963,24 +1909,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="14" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2014,15 +1942,6 @@
     <xf numFmtId="164" fontId="6" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2086,12 +2005,6 @@
     <xf numFmtId="1" fontId="6" fillId="2" borderId="22" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2128,28 +2041,7 @@
     <xf numFmtId="164" fontId="9" fillId="2" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2171,13 +2063,67 @@
     <xf numFmtId="2" fontId="9" fillId="2" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="2" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="2" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2186,47 +2132,104 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="2" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="2" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2664,1723 +2667,1730 @@
   </sheetPr>
   <dimension ref="B1:U101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="29" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.140625" style="29" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="29" customWidth="1"/>
-    <col min="6" max="6" width="48.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.7109375" style="29" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" style="29" customWidth="1"/>
-    <col min="10" max="10" width="3.5703125" style="29" customWidth="1"/>
-    <col min="11" max="14" width="19.140625" style="29" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="29" customWidth="1"/>
-    <col min="16" max="16" width="41.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="10.7109375" style="29" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="29"/>
+    <col min="1" max="1" width="7.33203125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="48.5" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.1640625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="28" customWidth="1"/>
+    <col min="6" max="6" width="48.6640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.6640625" style="28" customWidth="1"/>
+    <col min="9" max="9" width="7.1640625" style="28" customWidth="1"/>
+    <col min="10" max="10" width="3.5" style="28" customWidth="1"/>
+    <col min="11" max="14" width="19.1640625" style="28" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" style="28" customWidth="1"/>
+    <col min="16" max="16" width="41.6640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.6640625" style="28" customWidth="1"/>
+    <col min="20" max="16384" width="9.1640625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+    <row r="2" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="193" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="K2" s="31" t="s">
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="K2" s="166" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="33"/>
-      <c r="P2" s="34" t="s">
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="168"/>
+      <c r="P2" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="36"/>
-    </row>
-    <row r="3" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+      <c r="Q2" s="195"/>
+      <c r="R2" s="195"/>
+      <c r="S2" s="195"/>
+      <c r="T2" s="196"/>
+    </row>
+    <row r="3" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="197" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="40" t="s">
+      <c r="C3" s="183"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="41" t="s">
+      <c r="N3" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-    </row>
-    <row r="4" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+    </row>
+    <row r="4" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="183" t="s">
         <v>149</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="K4" s="43" t="s">
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
+      <c r="K4" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="44"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="46"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
-    </row>
-    <row r="5" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="38" t="s">
+      <c r="L4" s="34"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="36"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+    </row>
+    <row r="5" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="183" t="s">
         <v>153</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="K5" s="43" t="s">
+      <c r="C5" s="183"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="183"/>
+      <c r="G5" s="183"/>
+      <c r="H5" s="183"/>
+      <c r="K5" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="46"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-    </row>
-    <row r="6" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="38" t="s">
+      <c r="L5" s="34"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="36"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+    </row>
+    <row r="6" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="183" t="s">
         <v>154</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="K6" s="47" t="s">
+      <c r="C6" s="183"/>
+      <c r="D6" s="183"/>
+      <c r="E6" s="183"/>
+      <c r="F6" s="183"/>
+      <c r="G6" s="183"/>
+      <c r="H6" s="183"/>
+      <c r="K6" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="44"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="46"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-    </row>
-    <row r="7" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="38" t="s">
+      <c r="L6" s="34"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="36"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+    </row>
+    <row r="7" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="183" t="s">
         <v>152</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="K7" s="47" t="s">
+      <c r="C7" s="183"/>
+      <c r="D7" s="183"/>
+      <c r="E7" s="183"/>
+      <c r="F7" s="183"/>
+      <c r="G7" s="183"/>
+      <c r="H7" s="183"/>
+      <c r="K7" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="L7" s="44"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="46"/>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="42"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-    </row>
-    <row r="8" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K8" s="48" t="s">
+      <c r="L7" s="34"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="36"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+    </row>
+    <row r="8" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="49"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="51"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="42"/>
-    </row>
-    <row r="9" spans="2:21" s="56" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="52" t="s">
+      <c r="L8" s="39"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="41"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
+    </row>
+    <row r="9" spans="2:21" s="43" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="184" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="52" t="s">
+      <c r="C9" s="185"/>
+      <c r="D9" s="186"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="184" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="53"/>
-      <c r="H9" s="54"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="42"/>
-      <c r="S9" s="42"/>
-      <c r="T9" s="42"/>
-      <c r="U9" s="29"/>
-    </row>
-    <row r="10" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="57"/>
-      <c r="C10" s="58" t="s">
+      <c r="G9" s="185"/>
+      <c r="H9" s="186"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="28"/>
+    </row>
+    <row r="10" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="44"/>
+      <c r="C10" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="60"/>
-      <c r="G10" s="58" t="s">
+      <c r="F10" s="47"/>
+      <c r="G10" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="59" t="s">
+      <c r="H10" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="56"/>
-      <c r="K10" s="61" t="s">
+      <c r="J10" s="43"/>
+      <c r="K10" s="187" t="s">
         <v>55</v>
       </c>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="64" t="s">
+      <c r="L10" s="188"/>
+      <c r="M10" s="188"/>
+      <c r="N10" s="189"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="Q10" s="65" t="s">
+      <c r="Q10" s="49" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="66" t="s">
+    <row r="11" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="67">
+      <c r="C11" s="51">
         <f>'IPs From 2019 SAE Pub'!C13</f>
         <v>187</v>
       </c>
-      <c r="D11" s="68">
+      <c r="D11" s="52">
         <v>4</v>
       </c>
-      <c r="F11" s="69" t="s">
+      <c r="F11" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="70" t="s">
+      <c r="G11" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="H11" s="71" t="s">
+      <c r="H11" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="72" t="s">
+      <c r="K11" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="L11" s="73">
+      <c r="L11" s="190">
         <v>40179</v>
       </c>
-      <c r="M11" s="74"/>
-      <c r="N11" s="75"/>
-      <c r="P11" s="76" t="s">
+      <c r="M11" s="191"/>
+      <c r="N11" s="192"/>
+      <c r="P11" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="Q11" s="77">
+      <c r="Q11" s="58">
         <f>1/25.4</f>
         <v>3.937007874015748E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="66" t="s">
+    <row r="12" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="67">
+      <c r="C12" s="51">
         <f>'IPs From 2019 SAE Pub'!C14</f>
         <v>70</v>
       </c>
-      <c r="D12" s="68">
+      <c r="D12" s="52">
         <v>4</v>
       </c>
-      <c r="F12" s="78" t="s">
+      <c r="F12" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="79">
+      <c r="G12" s="60">
         <f>'IPs From 2019 SAE Pub'!C10</f>
         <v>3298</v>
       </c>
-      <c r="H12" s="80" t="s">
+      <c r="H12" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="81" t="s">
+      <c r="K12" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="L12" s="82">
+      <c r="L12" s="63">
         <v>36892</v>
       </c>
-      <c r="M12" s="82">
+      <c r="M12" s="63">
         <f ca="1">TODAY()</f>
-        <v>44043</v>
-      </c>
-      <c r="N12" s="83">
+        <v>44216</v>
+      </c>
+      <c r="N12" s="64">
         <v>26872</v>
       </c>
-      <c r="P12" s="84" t="s">
+      <c r="P12" s="65" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="66" t="s">
+    <row r="13" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="67">
+      <c r="C13" s="51">
         <f>'IPs From 2019 SAE Pub'!C15</f>
         <v>56.25</v>
       </c>
-      <c r="D13" s="68">
+      <c r="D13" s="52">
         <v>4</v>
       </c>
-      <c r="F13" s="66" t="s">
+      <c r="F13" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="85">
+      <c r="G13" s="66">
         <f>'IPs From 2019 SAE Pub'!C11</f>
         <v>0.64038811400848994</v>
       </c>
-      <c r="H13" s="68" t="s">
+      <c r="H13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="86" t="s">
+      <c r="K13" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="L13" s="87">
+      <c r="L13" s="68">
         <f>DATEDIF(L12,L11,"y")</f>
         <v>9</v>
       </c>
-      <c r="M13" s="87" t="e">
+      <c r="M13" s="68" t="e">
         <f ca="1">DATEDIF(M12,L11,"y")</f>
         <v>#NUM!</v>
       </c>
-      <c r="N13" s="88">
+      <c r="N13" s="69">
         <f>DATEDIF(N12,L11,"y")</f>
         <v>36</v>
       </c>
-      <c r="O13" s="89"/>
-      <c r="P13" s="90" t="s">
+      <c r="O13" s="70"/>
+      <c r="P13" s="71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="66" t="s">
+    <row r="14" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="67">
+      <c r="C14" s="51">
         <f>'IPs From 2019 SAE Pub'!C16</f>
         <v>106</v>
       </c>
-      <c r="D14" s="68">
+      <c r="D14" s="52">
         <v>4</v>
       </c>
-      <c r="F14" s="69" t="s">
+      <c r="F14" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="G14" s="91">
+      <c r="G14" s="72">
         <f>G13*G12</f>
         <v>2112</v>
       </c>
-      <c r="H14" s="92"/>
-      <c r="K14" s="93"/>
-      <c r="L14" s="93"/>
-      <c r="M14" s="93"/>
-    </row>
-    <row r="15" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="66" t="s">
+      <c r="H14" s="73"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="74"/>
+    </row>
+    <row r="15" spans="2:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="67">
+      <c r="C15" s="51">
         <f>'IPs From 2019 SAE Pub'!C17</f>
         <v>38</v>
       </c>
-      <c r="D15" s="68">
+      <c r="D15" s="52">
         <v>4</v>
       </c>
-      <c r="F15" s="94" t="s">
+      <c r="F15" s="75" t="s">
         <v>151</v>
       </c>
-      <c r="G15" s="95">
+      <c r="G15" s="76">
         <v>0</v>
       </c>
-      <c r="H15" s="96" t="s">
+      <c r="H15" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="31" t="s">
+      <c r="K15" s="166" t="s">
         <v>73</v>
       </c>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="33"/>
-    </row>
-    <row r="16" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="66" t="s">
+      <c r="L15" s="167"/>
+      <c r="M15" s="167"/>
+      <c r="N15" s="168"/>
+    </row>
+    <row r="16" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="67">
+      <c r="C16" s="51">
         <f>'IPs From 2019 SAE Pub'!C18</f>
         <v>60</v>
       </c>
-      <c r="D16" s="68">
+      <c r="D16" s="52">
         <v>4</v>
       </c>
-      <c r="F16" s="97"/>
-      <c r="G16" s="95"/>
-      <c r="H16" s="80"/>
-      <c r="K16" s="98" t="s">
+      <c r="F16" s="78"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="61"/>
+      <c r="K16" s="79" t="s">
         <v>75</v>
       </c>
-      <c r="L16" s="99" t="s">
+      <c r="L16" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="M16" s="99" t="s">
+      <c r="M16" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="N16" s="100" t="s">
+      <c r="N16" s="81" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="101" t="s">
+    <row r="17" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="67">
+      <c r="C17" s="51">
         <f>'IPs From 2019 SAE Pub'!C19</f>
         <v>59</v>
       </c>
-      <c r="D17" s="102">
+      <c r="D17" s="83">
         <v>4</v>
       </c>
-      <c r="F17" s="103"/>
-      <c r="G17" s="104"/>
-      <c r="H17" s="68"/>
-      <c r="K17" s="81" t="s">
+      <c r="F17" s="84"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="52"/>
+      <c r="K17" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="L17" s="105">
+      <c r="L17" s="86">
         <f>N17/C$14</f>
         <v>0</v>
       </c>
-      <c r="M17" s="106">
+      <c r="M17" s="87">
         <f>1-L17</f>
         <v>1</v>
       </c>
-      <c r="N17" s="68">
+      <c r="N17" s="52">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="107" t="s">
+    <row r="18" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="108" t="s">
+      <c r="C18" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="109" t="s">
+      <c r="D18" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="103"/>
-      <c r="G18" s="104"/>
-      <c r="H18" s="68"/>
-      <c r="K18" s="81" t="s">
+      <c r="F18" s="84"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="52"/>
+      <c r="K18" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="L18" s="105">
+      <c r="L18" s="86">
         <f>N18/C$14</f>
         <v>0</v>
       </c>
-      <c r="M18" s="106">
+      <c r="M18" s="87">
         <f>1-L18</f>
         <v>1</v>
       </c>
-      <c r="N18" s="68">
+      <c r="N18" s="52">
         <v>0</v>
       </c>
-      <c r="P18" s="110" t="s">
+      <c r="P18" s="169" t="s">
         <v>85</v>
       </c>
-      <c r="Q18" s="111"/>
-      <c r="R18" s="111"/>
-      <c r="S18" s="112"/>
-    </row>
-    <row r="19" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="66" t="s">
+      <c r="Q18" s="170"/>
+      <c r="R18" s="170"/>
+      <c r="S18" s="171"/>
+    </row>
+    <row r="19" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="95">
+      <c r="C19" s="76">
         <f>'IPs From 2019 SAE Pub'!C28</f>
         <v>215</v>
       </c>
-      <c r="D19" s="68">
+      <c r="D19" s="52">
         <v>215</v>
       </c>
-      <c r="F19" s="103"/>
-      <c r="G19" s="104"/>
-      <c r="H19" s="68"/>
-      <c r="K19" s="81" t="s">
+      <c r="F19" s="84"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="52"/>
+      <c r="K19" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="L19" s="105">
+      <c r="L19" s="86">
         <f>N19/C$14</f>
         <v>0</v>
       </c>
-      <c r="M19" s="106">
+      <c r="M19" s="87">
         <f>1-L19</f>
         <v>1</v>
       </c>
-      <c r="N19" s="68">
+      <c r="N19" s="52">
         <v>0</v>
       </c>
-      <c r="P19" s="113" t="s">
+      <c r="P19" s="172" t="s">
         <v>88</v>
       </c>
-      <c r="Q19" s="114"/>
-      <c r="R19" s="114"/>
-      <c r="S19" s="115"/>
-    </row>
-    <row r="20" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="66" t="s">
+      <c r="Q19" s="173"/>
+      <c r="R19" s="173"/>
+      <c r="S19" s="174"/>
+    </row>
+    <row r="20" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="95">
+      <c r="C20" s="76">
         <f>'IPs From 2019 SAE Pub'!C29</f>
         <v>60</v>
       </c>
-      <c r="D20" s="68">
+      <c r="D20" s="52">
         <v>60</v>
       </c>
-      <c r="F20" s="103"/>
-      <c r="G20" s="104"/>
-      <c r="H20" s="68"/>
-      <c r="K20" s="86" t="s">
+      <c r="F20" s="84"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="52"/>
+      <c r="K20" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="L20" s="116">
+      <c r="L20" s="91">
         <f>N20/C$14</f>
         <v>0</v>
       </c>
-      <c r="M20" s="117">
+      <c r="M20" s="92">
         <f>1-L20</f>
         <v>1</v>
       </c>
-      <c r="N20" s="71">
+      <c r="N20" s="55">
         <v>0</v>
       </c>
-      <c r="P20" s="118"/>
-      <c r="Q20" s="119" t="s">
+      <c r="P20" s="93"/>
+      <c r="Q20" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="R20" s="119" t="s">
+      <c r="R20" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="S20" s="120" t="s">
+      <c r="S20" s="95" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="66" t="s">
+    <row r="21" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="95">
+      <c r="C21" s="76">
         <f>'IPs From 2019 SAE Pub'!C30</f>
         <v>16</v>
       </c>
-      <c r="D21" s="68">
+      <c r="D21" s="52">
         <v>16</v>
       </c>
-      <c r="F21" s="103"/>
-      <c r="G21" s="104"/>
-      <c r="H21" s="68"/>
-      <c r="P21" s="121" t="s">
+      <c r="F21" s="84"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="52"/>
+      <c r="P21" s="96" t="s">
         <v>93</v>
       </c>
-      <c r="Q21" s="122">
+      <c r="Q21" s="97">
         <f>G29</f>
         <v>38.118859915100067</v>
       </c>
-      <c r="R21" s="122">
+      <c r="R21" s="97">
         <f>-(C16/2)</f>
         <v>-30</v>
       </c>
-      <c r="S21" s="123">
+      <c r="S21" s="98">
         <f>G30-(C22/2)</f>
         <v>8.4018473425196838</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="124" t="s">
+    <row r="22" spans="2:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="125">
+      <c r="C22" s="100">
         <f>C19*((C20/100)*2)/25.4+C21</f>
         <v>26.15748031496063</v>
       </c>
-      <c r="D22" s="126">
+      <c r="D22" s="101">
         <f>D19*((D20/100)*2)/25.4+D21</f>
         <v>26.15748031496063</v>
       </c>
-      <c r="F22" s="103"/>
-      <c r="G22" s="104"/>
-      <c r="H22" s="68"/>
-      <c r="K22" s="127" t="s">
+      <c r="F22" s="84"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="52"/>
+      <c r="K22" s="175" t="s">
         <v>95</v>
       </c>
-      <c r="L22" s="128"/>
-      <c r="M22" s="129"/>
-      <c r="P22" s="121" t="s">
+      <c r="L22" s="176"/>
+      <c r="M22" s="177"/>
+      <c r="P22" s="96" t="s">
         <v>96</v>
       </c>
-      <c r="Q22" s="122">
+      <c r="Q22" s="97">
         <f>G29</f>
         <v>38.118859915100067</v>
       </c>
-      <c r="R22" s="130">
+      <c r="R22" s="102">
         <f>C16/2</f>
         <v>30</v>
       </c>
-      <c r="S22" s="123">
+      <c r="S22" s="98">
         <f>G30-(C22/2)</f>
         <v>8.4018473425196838</v>
       </c>
     </row>
-    <row r="23" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="131" t="s">
+    <row r="23" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="132">
+      <c r="C23" s="104">
         <f>C19/25.4</f>
         <v>8.4645669291338592</v>
       </c>
-      <c r="D23" s="133">
+      <c r="D23" s="105">
         <f>D19/25.4</f>
         <v>8.4645669291338592</v>
       </c>
-      <c r="F23" s="103"/>
-      <c r="G23" s="104"/>
-      <c r="H23" s="68"/>
-      <c r="K23" s="134" t="s">
+      <c r="F23" s="84"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="52"/>
+      <c r="K23" s="106" t="s">
         <v>98</v>
       </c>
-      <c r="L23" s="135" t="s">
+      <c r="L23" s="107" t="s">
         <v>99</v>
       </c>
-      <c r="M23" s="136" t="s">
+      <c r="M23" s="108" t="s">
         <v>100</v>
       </c>
-      <c r="P23" s="121" t="s">
+      <c r="P23" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="Q23" s="130">
+      <c r="Q23" s="102">
         <f>-(C14-G29)</f>
         <v>-67.881140084899926</v>
       </c>
-      <c r="R23" s="130">
+      <c r="R23" s="102">
         <f>-(C17/2)</f>
         <v>-29.5</v>
       </c>
-      <c r="S23" s="123">
+      <c r="S23" s="98">
         <f>G30-(C22/2)</f>
         <v>8.4018473425196838</v>
       </c>
     </row>
-    <row r="24" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="107" t="s">
+    <row r="24" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="88" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="108" t="s">
+      <c r="C24" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="109" t="s">
+      <c r="D24" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="F24" s="69" t="s">
+      <c r="F24" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="G24" s="137">
+      <c r="G24" s="109">
         <f>SUM(G15:G23)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="138"/>
-      <c r="K24" s="134" t="s">
+      <c r="H24" s="110"/>
+      <c r="K24" s="106" t="s">
         <v>104</v>
       </c>
-      <c r="L24" s="139">
+      <c r="L24" s="111">
         <v>11.7</v>
       </c>
-      <c r="M24" s="140">
+      <c r="M24" s="112">
         <v>10.4</v>
       </c>
-      <c r="P24" s="141" t="s">
+      <c r="P24" s="113" t="s">
         <v>105</v>
       </c>
-      <c r="Q24" s="142">
+      <c r="Q24" s="114">
         <f>-(C14-G29)</f>
         <v>-67.881140084899926</v>
       </c>
-      <c r="R24" s="142">
+      <c r="R24" s="114">
         <f>C17/2</f>
         <v>29.5</v>
       </c>
-      <c r="S24" s="143">
+      <c r="S24" s="115">
         <f>G30-(C22/2)</f>
         <v>8.4018473425196838</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="66" t="s">
+    <row r="25" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="95">
+      <c r="C25" s="76">
         <v>215</v>
       </c>
-      <c r="D25" s="68">
+      <c r="D25" s="52">
         <v>215</v>
       </c>
-      <c r="F25" s="144" t="s">
+      <c r="F25" s="116" t="s">
         <v>106</v>
       </c>
-      <c r="G25" s="145"/>
-      <c r="H25" s="146"/>
-      <c r="K25" s="134" t="s">
+      <c r="G25" s="117"/>
+      <c r="H25" s="118"/>
+      <c r="K25" s="106" t="s">
         <v>107</v>
       </c>
-      <c r="L25" s="139">
+      <c r="L25" s="111">
         <v>16</v>
       </c>
-      <c r="M25" s="140">
+      <c r="M25" s="112">
         <v>14.7</v>
       </c>
-      <c r="P25" s="147"/>
-      <c r="Q25" s="148"/>
-      <c r="R25" s="148"/>
-      <c r="S25" s="149"/>
-      <c r="T25" s="56"/>
-    </row>
-    <row r="26" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="66" t="s">
+      <c r="P25" s="119"/>
+      <c r="Q25" s="120"/>
+      <c r="R25" s="120"/>
+      <c r="S25" s="121"/>
+      <c r="T25" s="43"/>
+    </row>
+    <row r="26" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="95">
+      <c r="C26" s="76">
         <v>60</v>
       </c>
-      <c r="D26" s="68">
+      <c r="D26" s="52">
         <v>60</v>
       </c>
-      <c r="F26" s="107" t="s">
+      <c r="F26" s="88" t="s">
         <v>109</v>
       </c>
-      <c r="G26" s="150">
+      <c r="G26" s="122">
         <f>G12+G24+G25</f>
         <v>3298</v>
       </c>
-      <c r="H26" s="59"/>
-      <c r="K26" s="134" t="s">
+      <c r="H26" s="46"/>
+      <c r="K26" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="L26" s="139">
+      <c r="L26" s="111">
         <v>18.5</v>
       </c>
-      <c r="M26" s="140">
+      <c r="M26" s="112">
         <v>17.2</v>
       </c>
-      <c r="P26" s="151" t="s">
+      <c r="P26" s="178" t="s">
         <v>42</v>
       </c>
-      <c r="Q26" s="152"/>
-      <c r="R26" s="148"/>
-      <c r="S26" s="153"/>
-    </row>
-    <row r="27" spans="2:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="66" t="s">
+      <c r="Q26" s="179"/>
+      <c r="R26" s="120"/>
+      <c r="S26" s="123"/>
+    </row>
+    <row r="27" spans="2:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="C27" s="95">
+      <c r="C27" s="76">
         <v>16</v>
       </c>
-      <c r="D27" s="68">
+      <c r="D27" s="52">
         <v>16</v>
       </c>
-      <c r="F27" s="66" t="s">
+      <c r="F27" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="G27" s="154">
+      <c r="G27" s="124">
         <f>G14+SUM(G15:G17)*L17+SUM(G18:G20)*L18+SUM(G21:G23)*L19+G25*L20</f>
         <v>2112</v>
       </c>
-      <c r="H27" s="155"/>
-      <c r="K27" s="134" t="s">
+      <c r="H27" s="125"/>
+      <c r="K27" s="106" t="s">
         <v>112</v>
       </c>
-      <c r="L27" s="139">
+      <c r="L27" s="111">
         <v>21</v>
       </c>
-      <c r="M27" s="140">
+      <c r="M27" s="112">
         <v>20.100000000000001</v>
       </c>
-      <c r="P27" s="156" t="s">
+      <c r="P27" s="126" t="s">
         <v>113</v>
       </c>
-      <c r="Q27" s="198">
+      <c r="Q27" s="157">
         <v>5</v>
       </c>
-      <c r="R27" s="148"/>
-      <c r="S27" s="153"/>
-    </row>
-    <row r="28" spans="2:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="124" t="s">
+      <c r="R27" s="120"/>
+      <c r="S27" s="123"/>
+    </row>
+    <row r="28" spans="2:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="125">
+      <c r="C28" s="100">
         <f>C25*((C26/100)*2)/25.4+C27</f>
         <v>26.15748031496063</v>
       </c>
-      <c r="D28" s="126">
+      <c r="D28" s="101">
         <f>D25*((D26/100)*2)/25.4+D27</f>
         <v>26.15748031496063</v>
       </c>
-      <c r="F28" s="66" t="s">
+      <c r="F28" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="157">
+      <c r="G28" s="127">
         <f>G27/G26</f>
         <v>0.64038811400848994</v>
       </c>
-      <c r="H28" s="158"/>
-      <c r="K28" s="134">
+      <c r="H28" s="128"/>
+      <c r="K28" s="106">
         <v>1</v>
       </c>
-      <c r="L28" s="139">
+      <c r="L28" s="111">
         <v>24.9</v>
       </c>
-      <c r="M28" s="140">
+      <c r="M28" s="112">
         <v>24.4</v>
       </c>
-      <c r="P28" s="121" t="s">
+      <c r="P28" s="96" t="s">
         <v>115</v>
       </c>
-      <c r="Q28" s="123">
+      <c r="Q28" s="98">
         <f>G29+C15</f>
         <v>76.118859915100074</v>
       </c>
-      <c r="R28" s="148"/>
-      <c r="S28" s="153"/>
-    </row>
-    <row r="29" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="159" t="s">
+      <c r="R28" s="120"/>
+      <c r="S28" s="123"/>
+    </row>
+    <row r="29" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="129" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="160">
+      <c r="C29" s="130">
         <f>C25/25.4</f>
         <v>8.4645669291338592</v>
       </c>
-      <c r="D29" s="161">
+      <c r="D29" s="131">
         <f>D25/25.4</f>
         <v>8.4645669291338592</v>
       </c>
-      <c r="F29" s="66" t="s">
+      <c r="F29" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="G29" s="162">
+      <c r="G29" s="132">
         <f>C14*(1-G28)</f>
         <v>38.118859915100067</v>
       </c>
-      <c r="H29" s="163"/>
-      <c r="K29" s="134">
+      <c r="H29" s="133"/>
+      <c r="K29" s="106">
         <v>2</v>
       </c>
-      <c r="L29" s="139">
+      <c r="L29" s="111">
         <v>30.8</v>
       </c>
-      <c r="M29" s="140">
+      <c r="M29" s="112">
         <v>28.8</v>
       </c>
-      <c r="P29" s="121" t="s">
+      <c r="P29" s="96" t="s">
         <v>117</v>
       </c>
-      <c r="Q29" s="123">
+      <c r="Q29" s="98">
         <f>Q28-C11</f>
         <v>-110.88114008489993</v>
       </c>
-      <c r="R29" s="148"/>
-      <c r="S29" s="153"/>
-    </row>
-    <row r="30" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F30" s="66" t="s">
+      <c r="R29" s="120"/>
+      <c r="S29" s="123"/>
+    </row>
+    <row r="30" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="G30" s="162">
+      <c r="G30" s="132">
         <f>AVERAGE(0.3891*C13+0.0113,IF(G11="Fwd-Car",21.063,IF(G11="Rwd-Car",0.39*C13,IF(G11="Pickup",0.376*C13,IF(G11="SUV",0.39*C13,IF(G11="Van",0.381*C13,""))))))</f>
         <v>21.480587499999999</v>
       </c>
-      <c r="H30" s="155">
+      <c r="H30" s="125">
         <f>D36</f>
         <v>5</v>
       </c>
-      <c r="K30" s="134">
+      <c r="K30" s="106">
         <v>3</v>
       </c>
-      <c r="L30" s="139">
+      <c r="L30" s="111">
         <v>34.6</v>
       </c>
-      <c r="M30" s="140">
+      <c r="M30" s="112">
         <v>33.4</v>
       </c>
-      <c r="P30" s="121" t="s">
+      <c r="P30" s="96" t="s">
         <v>119</v>
       </c>
-      <c r="Q30" s="164">
+      <c r="Q30" s="134">
         <f>-C12/2</f>
         <v>-35</v>
       </c>
-      <c r="R30" s="148"/>
-      <c r="S30" s="153"/>
-    </row>
-    <row r="31" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="165" t="s">
+      <c r="R30" s="120"/>
+      <c r="S30" s="123"/>
+    </row>
+    <row r="31" spans="2:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="180" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="166"/>
-      <c r="D31" s="167"/>
-      <c r="F31" s="66" t="s">
+      <c r="C31" s="181"/>
+      <c r="D31" s="182"/>
+      <c r="F31" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="G31" s="154">
+      <c r="G31" s="124">
         <f>AVERAGE((10^-2.1363*(C14/12)^-0.1596*(((C16+C17)/2)/12)^1.9404*(C13/12)^0.3629*G26^0.9421),IF(G11="Fwd-Car",(0.1274*(G26*4.448/9.81)*((C13+535/25.4)/(12*3.2808))*(((C16+C17)/2)/(12*3.2808)))/1.356,IF(G11="Rwd-Car",(0.12*(G26*4.448/9.81)*((C13+0.39*C13)/(12*3.2808))*(((C16+C17)/2)/(12*3.2808)))/1.356,IF(G11="Pickup",(0.138*(G26*4.448/9.81)*(((C16+C17)/2)/(12*3.2808))*(C13/(12*3.2808)))/1.356,IF(G11="SUV",(0.145*(G26*4.448/9.81)*(((C16+C17)/2)/(12*3.2808))*(C13/(12*3.2808)))/1.356,IF(G11="Van",(0.1212*(G26*4.448/9.81)*((C13+0.381*C13)/(12*3.2808))*(((C16+C17)/2)/(12*3.2808)))/1.356,""))))))</f>
         <v>416.89822232506287</v>
       </c>
-      <c r="H31" s="155">
+      <c r="H31" s="125">
         <f>D36</f>
         <v>5</v>
       </c>
-      <c r="K31" s="134">
+      <c r="K31" s="106">
         <v>4</v>
       </c>
-      <c r="L31" s="139">
+      <c r="L31" s="111">
         <v>39.799999999999997</v>
       </c>
-      <c r="M31" s="140">
+      <c r="M31" s="112">
         <v>39.5</v>
       </c>
-      <c r="P31" s="121" t="s">
+      <c r="P31" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="Q31" s="164">
+      <c r="Q31" s="134">
         <f>C12/2</f>
         <v>35</v>
       </c>
-      <c r="R31" s="148"/>
-      <c r="S31" s="153"/>
-    </row>
-    <row r="32" spans="2:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="168" t="s">
+      <c r="R31" s="120"/>
+      <c r="S31" s="123"/>
+    </row>
+    <row r="32" spans="2:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="158" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="169"/>
-      <c r="D32" s="59">
+      <c r="C32" s="159"/>
+      <c r="D32" s="46">
         <v>1</v>
       </c>
-      <c r="F32" s="66" t="s">
+      <c r="F32" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="G32" s="154">
+      <c r="G32" s="124">
         <f>AVERAGE((10^-2.0024*(C14/12)^1.5315*(((C16+C17)/2)/12)^0.2526*(C13/12)^0.1009*G26^1.0206),IF(G11="Fwd-Car",(0.1425*(G26*4.448/9.81)*(C14/(12*3.2808))*((C11)/(12*3.2808)))/1.356,IF(G11="Rwd-Car",(0.0733*(G26*4.448/9.81)*((C11/(12*3.2808))^2+(C13/(12*3.2808))^2))/1.356,IF(G11="Pickup",(0.952*(G26*4.448/9.81)*(G29/(12*3.2808))*((C14-G29)/(12*3.2808)))/1.356,IF(G11="SUV",(0.1561*(G26*4.448/9.81)*(C14/(12*3.2808))*(C11/(12*3.2808)))/1.356,IF(G11="Van",(0.1508*(G26*4.448/9.81)*(C14/(12*3.2808))*(C11/(12*3.2808)))/1.356,""))))))</f>
         <v>1959.0114406803946</v>
       </c>
-      <c r="H32" s="155">
+      <c r="H32" s="125">
         <f>D36</f>
         <v>5</v>
       </c>
-      <c r="K32" s="134">
+      <c r="K32" s="106">
         <v>5</v>
       </c>
-      <c r="L32" s="139">
+      <c r="L32" s="111">
         <v>44.4</v>
       </c>
-      <c r="M32" s="140">
+      <c r="M32" s="112">
         <v>43.8</v>
       </c>
-      <c r="P32" s="121" t="s">
+      <c r="P32" s="96" t="s">
         <v>124</v>
       </c>
-      <c r="Q32" s="164">
+      <c r="Q32" s="134">
         <f>G30-Q27</f>
         <v>16.480587499999999</v>
       </c>
-      <c r="R32" s="148"/>
-      <c r="S32" s="170"/>
-    </row>
-    <row r="33" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="171" t="s">
+      <c r="R32" s="120"/>
+      <c r="S32" s="135"/>
+    </row>
+    <row r="33" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="160" t="s">
         <v>125</v>
       </c>
-      <c r="C33" s="172"/>
-      <c r="D33" s="173">
+      <c r="C33" s="161"/>
+      <c r="D33" s="136">
         <v>2</v>
       </c>
-      <c r="F33" s="69" t="s">
+      <c r="F33" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="G33" s="137">
+      <c r="G33" s="109">
         <f>AVERAGE((10^-1.7797*(C14/12)^1.4316*(((C16+C17)/2)/12)^0.3811*(C13/12)^0.0188*G26^0.98),IF(G11="Fwd-Car",(0.1478*(G26*4.448/9.81)*(C14/(12*3.2808))*((C11)/(12*3.2808)))/1.356,IF(G11="Rwd-Car",1.015*((2*(1-G28)*(G26*4.448/9.81)*(C11/(12*3.2808))^2/12)+(((2*G28)-1)*(G26*4.448/9.81)*(C14/(12*3.2808))^2/4))/1.356,IF(G11="Pickup",(0.958*(G26*4.448/9.81)*(G29/(12*3.2808))*((C14-G29)/(12*3.2808)))/1.356,IF(G11="SUV",(0.4622*(G26*4.448/9.81)*(((C16+C17)/2)/(12*3.2808))*(C14/(12*3.2808)))/1.356,IF(G11="Van",(0.1525*(G26*4.448/9.81)*(C14/(12*3.2808))*(C11/(12*3.2808)))/1.356,""))))))</f>
         <v>2040.4506492119394</v>
       </c>
-      <c r="H33" s="174">
+      <c r="H33" s="137">
         <f>D36</f>
         <v>5</v>
       </c>
-      <c r="K33" s="134">
+      <c r="K33" s="106">
         <v>6</v>
       </c>
-      <c r="L33" s="139">
+      <c r="L33" s="111">
         <v>50.8</v>
       </c>
-      <c r="M33" s="140">
+      <c r="M33" s="112">
         <v>49</v>
       </c>
-      <c r="P33" s="141" t="s">
+      <c r="P33" s="113" t="s">
         <v>127</v>
       </c>
-      <c r="Q33" s="175">
+      <c r="Q33" s="138">
         <f>-(C13-G30)</f>
         <v>-34.769412500000001</v>
       </c>
-      <c r="R33" s="148"/>
-      <c r="S33" s="170"/>
-    </row>
-    <row r="34" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="171" t="s">
+      <c r="R33" s="120"/>
+      <c r="S33" s="135"/>
+    </row>
+    <row r="34" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="160" t="s">
         <v>128</v>
       </c>
-      <c r="C34" s="172"/>
-      <c r="D34" s="173">
+      <c r="C34" s="161"/>
+      <c r="D34" s="136">
         <v>3</v>
       </c>
-      <c r="F34" s="176"/>
-      <c r="G34" s="176"/>
-      <c r="H34" s="176"/>
-      <c r="K34" s="134">
+      <c r="F34" s="139"/>
+      <c r="G34" s="139"/>
+      <c r="H34" s="139"/>
+      <c r="K34" s="106">
         <v>7</v>
       </c>
-      <c r="L34" s="139">
+      <c r="L34" s="111">
         <v>57.4</v>
       </c>
-      <c r="M34" s="140">
+      <c r="M34" s="112">
         <v>53.9</v>
       </c>
-      <c r="P34" s="177" t="s">
+      <c r="P34" s="140" t="s">
         <v>109</v>
       </c>
-      <c r="Q34" s="178">
+      <c r="Q34" s="141">
         <f>G26</f>
         <v>3298</v>
       </c>
-      <c r="R34" s="148"/>
-      <c r="S34" s="170"/>
-    </row>
-    <row r="35" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="171" t="s">
+      <c r="R34" s="120"/>
+      <c r="S34" s="135"/>
+    </row>
+    <row r="35" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="160" t="s">
         <v>129</v>
       </c>
-      <c r="C35" s="172"/>
-      <c r="D35" s="173">
+      <c r="C35" s="161"/>
+      <c r="D35" s="136">
         <v>4</v>
       </c>
-      <c r="F35" s="176"/>
-      <c r="G35" s="176"/>
-      <c r="H35" s="176"/>
-      <c r="K35" s="134">
+      <c r="F35" s="139"/>
+      <c r="G35" s="139"/>
+      <c r="H35" s="139"/>
+      <c r="K35" s="106">
         <v>8</v>
       </c>
-      <c r="L35" s="139">
+      <c r="L35" s="111">
         <v>65.5</v>
       </c>
-      <c r="M35" s="140">
+      <c r="M35" s="112">
         <v>63.3</v>
       </c>
-      <c r="P35" s="121" t="s">
+      <c r="P35" s="96" t="s">
         <v>130</v>
       </c>
-      <c r="Q35" s="179">
+      <c r="Q35" s="142">
         <f>Q34/(32.17*12)</f>
         <v>8.5431561496218009</v>
       </c>
-      <c r="R35" s="148"/>
-      <c r="S35" s="170"/>
-    </row>
-    <row r="36" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="180" t="s">
+      <c r="R35" s="120"/>
+      <c r="S35" s="135"/>
+    </row>
+    <row r="36" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="162" t="s">
         <v>131</v>
       </c>
-      <c r="C36" s="181"/>
-      <c r="D36" s="182">
+      <c r="C36" s="163"/>
+      <c r="D36" s="143">
         <v>5</v>
       </c>
-      <c r="F36" s="176"/>
-      <c r="G36" s="176"/>
-      <c r="H36" s="176"/>
-      <c r="K36" s="134">
+      <c r="F36" s="139"/>
+      <c r="G36" s="139"/>
+      <c r="H36" s="139"/>
+      <c r="K36" s="106">
         <v>9</v>
       </c>
-      <c r="L36" s="139">
+      <c r="L36" s="111">
         <v>70.2</v>
       </c>
-      <c r="M36" s="140">
+      <c r="M36" s="112">
         <v>75.5</v>
       </c>
-      <c r="P36" s="121" t="s">
+      <c r="P36" s="96" t="s">
         <v>132</v>
       </c>
-      <c r="Q36" s="179">
+      <c r="Q36" s="142">
         <f>G31*12</f>
         <v>5002.778667900755</v>
       </c>
-      <c r="R36" s="148"/>
-      <c r="S36" s="170"/>
-    </row>
-    <row r="37" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F37" s="176"/>
-      <c r="G37" s="176"/>
-      <c r="H37" s="176"/>
-      <c r="K37" s="134">
+      <c r="R36" s="120"/>
+      <c r="S36" s="135"/>
+    </row>
+    <row r="37" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F37" s="139"/>
+      <c r="G37" s="139"/>
+      <c r="H37" s="139"/>
+      <c r="K37" s="106">
         <v>10</v>
       </c>
-      <c r="L37" s="139">
+      <c r="L37" s="111">
         <v>80.5</v>
       </c>
-      <c r="M37" s="140">
+      <c r="M37" s="112">
         <v>85.3</v>
       </c>
-      <c r="P37" s="121" t="s">
+      <c r="P37" s="96" t="s">
         <v>133</v>
       </c>
-      <c r="Q37" s="179">
+      <c r="Q37" s="142">
         <f>G32*12</f>
         <v>23508.137288164733</v>
       </c>
-      <c r="R37" s="148"/>
-      <c r="S37" s="170"/>
-    </row>
-    <row r="38" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F38" s="176"/>
-      <c r="G38" s="176"/>
-      <c r="H38" s="176"/>
-      <c r="K38" s="134">
+      <c r="R37" s="120"/>
+      <c r="S37" s="135"/>
+    </row>
+    <row r="38" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="F38" s="139"/>
+      <c r="G38" s="139"/>
+      <c r="H38" s="139"/>
+      <c r="K38" s="106">
         <v>11</v>
       </c>
-      <c r="L38" s="139">
+      <c r="L38" s="111">
         <v>100.9</v>
       </c>
-      <c r="M38" s="140">
+      <c r="M38" s="112">
         <v>97</v>
       </c>
-      <c r="P38" s="121" t="s">
+      <c r="P38" s="96" t="s">
         <v>134</v>
       </c>
-      <c r="Q38" s="179">
+      <c r="Q38" s="142">
         <f>G33*12</f>
         <v>24485.407790543271</v>
       </c>
-      <c r="R38" s="148"/>
-      <c r="S38" s="170"/>
-    </row>
-    <row r="39" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="183" t="s">
+      <c r="R38" s="120"/>
+      <c r="S38" s="135"/>
+    </row>
+    <row r="39" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="164" t="s">
         <v>135</v>
       </c>
-      <c r="C39" s="184"/>
-      <c r="F39" s="176"/>
-      <c r="G39" s="176"/>
-      <c r="H39" s="176"/>
-      <c r="K39" s="134">
+      <c r="C39" s="165"/>
+      <c r="F39" s="139"/>
+      <c r="G39" s="139"/>
+      <c r="H39" s="139"/>
+      <c r="K39" s="106">
         <v>12</v>
       </c>
-      <c r="L39" s="139">
+      <c r="L39" s="111">
         <v>105</v>
       </c>
-      <c r="M39" s="140">
+      <c r="M39" s="112">
         <v>112.2</v>
       </c>
-      <c r="P39" s="141" t="s">
+      <c r="P39" s="113" t="s">
         <v>118</v>
       </c>
-      <c r="Q39" s="185">
+      <c r="Q39" s="144">
         <f>G30</f>
         <v>21.480587499999999</v>
       </c>
-      <c r="R39" s="186"/>
-      <c r="S39" s="187"/>
-    </row>
-    <row r="40" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="188" t="s">
+      <c r="R39" s="145"/>
+      <c r="S39" s="146"/>
+    </row>
+    <row r="40" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="147" t="s">
         <v>136</v>
       </c>
-      <c r="C40" s="189">
+      <c r="C40" s="148">
         <f>C11</f>
         <v>187</v>
       </c>
-      <c r="F40" s="176"/>
-      <c r="G40" s="176"/>
-      <c r="H40" s="176"/>
-      <c r="K40" s="134">
+      <c r="F40" s="139"/>
+      <c r="G40" s="139"/>
+      <c r="H40" s="139"/>
+      <c r="K40" s="106">
         <v>13</v>
       </c>
-      <c r="L40" s="139">
+      <c r="L40" s="111">
         <v>125.1</v>
       </c>
-      <c r="M40" s="140">
+      <c r="M40" s="112">
         <v>113.2</v>
       </c>
     </row>
-    <row r="41" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="190" t="s">
+    <row r="41" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="149" t="s">
         <v>137</v>
       </c>
-      <c r="C41" s="191">
+      <c r="C41" s="150">
         <f t="shared" ref="C41:C42" si="0">C12</f>
         <v>70</v>
       </c>
-      <c r="F41" s="176"/>
-      <c r="G41" s="176"/>
-      <c r="H41" s="176"/>
-      <c r="K41" s="134">
+      <c r="F41" s="139"/>
+      <c r="G41" s="139"/>
+      <c r="H41" s="139"/>
+      <c r="K41" s="106">
         <v>14</v>
       </c>
-      <c r="L41" s="139">
+      <c r="L41" s="111">
         <v>135.4</v>
       </c>
-      <c r="M41" s="140">
+      <c r="M41" s="112">
         <v>118.5</v>
       </c>
     </row>
-    <row r="42" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="190" t="s">
+    <row r="42" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="149" t="s">
         <v>138</v>
       </c>
-      <c r="C42" s="191">
+      <c r="C42" s="150">
         <f t="shared" si="0"/>
         <v>56.25</v>
       </c>
-      <c r="F42" s="176"/>
-      <c r="G42" s="176"/>
-      <c r="H42" s="176"/>
-      <c r="K42" s="134">
+      <c r="F42" s="139"/>
+      <c r="G42" s="139"/>
+      <c r="H42" s="139"/>
+      <c r="K42" s="106">
         <v>15</v>
       </c>
-      <c r="L42" s="139">
+      <c r="L42" s="111">
         <v>144.5</v>
       </c>
-      <c r="M42" s="140">
+      <c r="M42" s="112">
         <v>128.1</v>
       </c>
-      <c r="O42" s="148"/>
-    </row>
-    <row r="43" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="190" t="s">
+      <c r="O42" s="120"/>
+    </row>
+    <row r="43" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="149" t="s">
         <v>139</v>
       </c>
-      <c r="C43" s="191">
+      <c r="C43" s="150">
         <f>G29+C15</f>
         <v>76.118859915100074</v>
       </c>
-      <c r="F43" s="176"/>
-      <c r="G43" s="176"/>
-      <c r="H43" s="176"/>
-      <c r="K43" s="134">
+      <c r="F43" s="139"/>
+      <c r="G43" s="139"/>
+      <c r="H43" s="139"/>
+      <c r="K43" s="106">
         <v>16</v>
       </c>
-      <c r="L43" s="139">
+      <c r="L43" s="111">
         <v>151.4</v>
       </c>
-      <c r="M43" s="140">
+      <c r="M43" s="112">
         <v>132.30000000000001</v>
       </c>
     </row>
-    <row r="44" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="190" t="s">
+    <row r="44" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="149" t="s">
         <v>118</v>
       </c>
-      <c r="C44" s="191">
+      <c r="C44" s="150">
         <f>G30</f>
         <v>21.480587499999999</v>
       </c>
-      <c r="F44" s="176"/>
-      <c r="G44" s="176"/>
-      <c r="H44" s="176"/>
-      <c r="K44" s="134">
+      <c r="F44" s="139"/>
+      <c r="G44" s="139"/>
+      <c r="H44" s="139"/>
+      <c r="K44" s="106">
         <v>17</v>
       </c>
-      <c r="L44" s="139">
+      <c r="L44" s="111">
         <v>156.80000000000001</v>
       </c>
-      <c r="M44" s="140">
+      <c r="M44" s="112">
         <v>133.80000000000001</v>
       </c>
     </row>
-    <row r="45" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="190" t="s">
+    <row r="45" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="149" t="s">
         <v>72</v>
       </c>
-      <c r="C45" s="191">
+      <c r="C45" s="150">
         <f>C15</f>
         <v>38</v>
       </c>
-      <c r="F45" s="176"/>
-      <c r="G45" s="176"/>
-      <c r="H45" s="176"/>
-      <c r="K45" s="134">
+      <c r="F45" s="139"/>
+      <c r="G45" s="139"/>
+      <c r="H45" s="139"/>
+      <c r="K45" s="106">
         <v>18</v>
       </c>
-      <c r="L45" s="139">
+      <c r="L45" s="111">
         <v>168.5</v>
       </c>
-      <c r="M45" s="140">
+      <c r="M45" s="112">
         <v>137</v>
       </c>
     </row>
-    <row r="46" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="190" t="s">
+    <row r="46" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="149" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="191">
+      <c r="C46" s="150">
         <f>C14</f>
         <v>106</v>
       </c>
-      <c r="F46" s="176"/>
-      <c r="G46" s="176"/>
-      <c r="H46" s="176"/>
-      <c r="K46" s="134">
+      <c r="F46" s="139"/>
+      <c r="G46" s="139"/>
+      <c r="H46" s="139"/>
+      <c r="K46" s="106">
         <v>19</v>
       </c>
-      <c r="L46" s="139">
+      <c r="L46" s="111">
         <v>162.5</v>
       </c>
-      <c r="M46" s="140">
+      <c r="M46" s="112">
         <v>137.9</v>
       </c>
     </row>
-    <row r="47" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="190" t="s">
+    <row r="47" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="149" t="s">
         <v>140</v>
       </c>
-      <c r="C47" s="191">
+      <c r="C47" s="150">
         <f>C22/2</f>
         <v>13.078740157480315</v>
       </c>
-      <c r="F47" s="176"/>
-      <c r="G47" s="176"/>
-      <c r="H47" s="176"/>
-      <c r="K47" s="134" t="s">
+      <c r="F47" s="139"/>
+      <c r="G47" s="139"/>
+      <c r="H47" s="139"/>
+      <c r="K47" s="106" t="s">
         <v>141</v>
       </c>
-      <c r="L47" s="139">
+      <c r="L47" s="111">
         <v>177.8</v>
       </c>
-      <c r="M47" s="140">
+      <c r="M47" s="112">
         <v>149.80000000000001</v>
       </c>
     </row>
-    <row r="48" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="190" t="s">
+    <row r="48" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="149" t="s">
         <v>142</v>
       </c>
-      <c r="C48" s="191">
+      <c r="C48" s="150">
         <f>C23</f>
         <v>8.4645669291338592</v>
       </c>
-      <c r="F48" s="176"/>
-      <c r="G48" s="176"/>
-      <c r="H48" s="176"/>
-      <c r="K48" s="134" t="s">
+      <c r="F48" s="139"/>
+      <c r="G48" s="139"/>
+      <c r="H48" s="139"/>
+      <c r="K48" s="106" t="s">
         <v>143</v>
       </c>
-      <c r="L48" s="139">
+      <c r="L48" s="111">
         <v>190.8</v>
       </c>
-      <c r="M48" s="140">
+      <c r="M48" s="112">
         <v>160.5</v>
       </c>
     </row>
-    <row r="49" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="190" t="s">
+    <row r="49" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="149" t="s">
         <v>74</v>
       </c>
-      <c r="C49" s="191">
+      <c r="C49" s="150">
         <f>C16</f>
         <v>60</v>
       </c>
-      <c r="F49" s="176"/>
-      <c r="G49" s="176"/>
-      <c r="H49" s="176"/>
-      <c r="K49" s="134" t="s">
+      <c r="F49" s="139"/>
+      <c r="G49" s="139"/>
+      <c r="H49" s="139"/>
+      <c r="K49" s="106" t="s">
         <v>144</v>
       </c>
-      <c r="L49" s="139">
+      <c r="L49" s="111">
         <v>196.4</v>
       </c>
-      <c r="M49" s="140">
+      <c r="M49" s="112">
         <v>164</v>
       </c>
     </row>
-    <row r="50" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="192" t="s">
+    <row r="50" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="151" t="s">
         <v>79</v>
       </c>
-      <c r="C50" s="193">
+      <c r="C50" s="152">
         <f>C17</f>
         <v>59</v>
       </c>
-      <c r="F50" s="176"/>
-      <c r="G50" s="176"/>
-      <c r="H50" s="176"/>
-      <c r="K50" s="134" t="s">
+      <c r="F50" s="139"/>
+      <c r="G50" s="139"/>
+      <c r="H50" s="139"/>
+      <c r="K50" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="L50" s="139">
+      <c r="L50" s="111">
         <v>195.9</v>
       </c>
-      <c r="M50" s="140">
+      <c r="M50" s="112">
         <v>167.4</v>
       </c>
     </row>
-    <row r="51" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F51" s="176"/>
-      <c r="G51" s="176"/>
-      <c r="H51" s="176"/>
-      <c r="K51" s="134" t="s">
+    <row r="51" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F51" s="139"/>
+      <c r="G51" s="139"/>
+      <c r="H51" s="139"/>
+      <c r="K51" s="106" t="s">
         <v>146</v>
       </c>
-      <c r="L51" s="139">
+      <c r="L51" s="111">
         <v>195.3</v>
       </c>
-      <c r="M51" s="140">
+      <c r="M51" s="112">
         <v>164.4</v>
       </c>
     </row>
-    <row r="52" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F52" s="176"/>
-      <c r="G52" s="176"/>
-      <c r="H52" s="176"/>
-      <c r="K52" s="134" t="s">
+    <row r="52" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F52" s="139"/>
+      <c r="G52" s="139"/>
+      <c r="H52" s="139"/>
+      <c r="K52" s="106" t="s">
         <v>147</v>
       </c>
-      <c r="L52" s="139">
+      <c r="L52" s="111">
         <v>183.6</v>
       </c>
-      <c r="M52" s="140">
+      <c r="M52" s="112">
         <v>158.5</v>
       </c>
     </row>
-    <row r="53" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F53" s="176"/>
-      <c r="G53" s="176"/>
-      <c r="H53" s="176"/>
-      <c r="K53" s="194" t="s">
+    <row r="53" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="F53" s="139"/>
+      <c r="G53" s="139"/>
+      <c r="H53" s="139"/>
+      <c r="K53" s="153" t="s">
         <v>148</v>
       </c>
-      <c r="L53" s="195">
+      <c r="L53" s="154">
         <v>171.1</v>
       </c>
-      <c r="M53" s="196">
+      <c r="M53" s="155">
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F54" s="176"/>
-      <c r="G54" s="176"/>
-      <c r="H54" s="176"/>
-    </row>
-    <row r="55" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F55" s="176"/>
-      <c r="G55" s="176"/>
-      <c r="H55" s="176"/>
-    </row>
-    <row r="56" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F56" s="176"/>
-      <c r="G56" s="176"/>
-      <c r="H56" s="176"/>
-    </row>
-    <row r="57" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F57" s="176"/>
-      <c r="G57" s="176"/>
-      <c r="H57" s="176"/>
-    </row>
-    <row r="58" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F58" s="176"/>
-      <c r="G58" s="176"/>
-      <c r="H58" s="176"/>
-    </row>
-    <row r="59" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F59" s="176"/>
-      <c r="G59" s="176"/>
-      <c r="H59" s="176"/>
-    </row>
-    <row r="60" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F60" s="176"/>
-      <c r="G60" s="176"/>
-      <c r="H60" s="176"/>
-    </row>
-    <row r="61" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F61" s="176"/>
-      <c r="G61" s="176"/>
-      <c r="H61" s="176"/>
-    </row>
-    <row r="62" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F62" s="176"/>
-      <c r="G62" s="176"/>
-      <c r="H62" s="176"/>
-    </row>
-    <row r="63" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F63" s="176"/>
-      <c r="G63" s="176"/>
-      <c r="H63" s="176"/>
-    </row>
-    <row r="64" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F64" s="176"/>
-      <c r="G64" s="176"/>
-      <c r="H64" s="176"/>
-    </row>
-    <row r="65" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F65" s="176"/>
-      <c r="G65" s="176"/>
-      <c r="H65" s="176"/>
-    </row>
-    <row r="66" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F66" s="176"/>
-      <c r="G66" s="176"/>
-      <c r="H66" s="176"/>
-    </row>
-    <row r="67" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F67" s="176"/>
-      <c r="G67" s="176"/>
-      <c r="H67" s="176"/>
-    </row>
-    <row r="68" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F68" s="176"/>
-      <c r="G68" s="176"/>
-      <c r="H68" s="176"/>
-    </row>
-    <row r="69" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F69" s="176"/>
-      <c r="G69" s="176"/>
-      <c r="H69" s="176"/>
-    </row>
-    <row r="70" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F70" s="176"/>
-      <c r="G70" s="176"/>
-      <c r="H70" s="176"/>
-    </row>
-    <row r="71" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F71" s="176"/>
-      <c r="G71" s="176"/>
-      <c r="H71" s="176"/>
-    </row>
-    <row r="72" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F72" s="176"/>
-      <c r="G72" s="176"/>
-      <c r="H72" s="176"/>
-    </row>
-    <row r="73" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F73" s="176"/>
-      <c r="G73" s="176"/>
-      <c r="H73" s="176"/>
-    </row>
-    <row r="74" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F74" s="176"/>
-      <c r="G74" s="176"/>
-      <c r="H74" s="176"/>
-    </row>
-    <row r="75" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F75" s="176"/>
-      <c r="G75" s="176"/>
-      <c r="H75" s="176"/>
-    </row>
-    <row r="76" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F76" s="176"/>
-      <c r="G76" s="176"/>
-      <c r="H76" s="176"/>
-      <c r="S76" s="89"/>
-    </row>
-    <row r="77" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F77" s="176"/>
-      <c r="G77" s="176"/>
-      <c r="H77" s="176"/>
-    </row>
-    <row r="78" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F78" s="176"/>
-      <c r="G78" s="176"/>
-      <c r="H78" s="176"/>
-    </row>
-    <row r="79" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F79" s="176"/>
-      <c r="G79" s="176"/>
-      <c r="H79" s="176"/>
-    </row>
-    <row r="80" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F80" s="176"/>
-      <c r="G80" s="176"/>
-      <c r="H80" s="176"/>
-    </row>
-    <row r="81" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F81" s="176"/>
-      <c r="G81" s="176"/>
-      <c r="H81" s="176"/>
-    </row>
-    <row r="82" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F82" s="176"/>
-      <c r="G82" s="176"/>
-      <c r="H82" s="176"/>
-    </row>
-    <row r="83" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F83" s="176"/>
-      <c r="G83" s="176"/>
-      <c r="H83" s="176"/>
-      <c r="Q83" s="197"/>
-    </row>
-    <row r="84" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F84" s="176"/>
-      <c r="G84" s="176"/>
-      <c r="H84" s="176"/>
-    </row>
-    <row r="85" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F85" s="176"/>
-      <c r="G85" s="176"/>
-      <c r="H85" s="176"/>
-    </row>
-    <row r="86" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F86" s="176"/>
-      <c r="G86" s="176"/>
-      <c r="H86" s="176"/>
-    </row>
-    <row r="87" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F87" s="176"/>
-      <c r="G87" s="176"/>
-      <c r="H87" s="176"/>
-    </row>
-    <row r="88" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F88" s="176"/>
-      <c r="G88" s="176"/>
-      <c r="H88" s="176"/>
-    </row>
-    <row r="89" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F89" s="176"/>
-      <c r="G89" s="176"/>
-      <c r="H89" s="176"/>
-    </row>
-    <row r="90" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F90" s="176"/>
-      <c r="G90" s="176"/>
-      <c r="H90" s="176"/>
-    </row>
-    <row r="91" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F91" s="176"/>
-      <c r="G91" s="176"/>
-      <c r="H91" s="176"/>
-    </row>
-    <row r="92" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F92" s="176"/>
-      <c r="G92" s="176"/>
-      <c r="H92" s="176"/>
-    </row>
-    <row r="93" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F93" s="176"/>
-      <c r="G93" s="176"/>
-      <c r="H93" s="176"/>
-    </row>
-    <row r="94" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F94" s="176"/>
-      <c r="G94" s="176"/>
-      <c r="H94" s="176"/>
-    </row>
-    <row r="95" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F95" s="176"/>
-      <c r="G95" s="176"/>
-      <c r="H95" s="176"/>
-    </row>
-    <row r="96" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F96" s="176"/>
-      <c r="G96" s="176"/>
-      <c r="H96" s="176"/>
-    </row>
-    <row r="97" spans="6:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F97" s="176"/>
-      <c r="G97" s="176"/>
-      <c r="H97" s="176"/>
-    </row>
-    <row r="98" spans="6:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F98" s="176"/>
-      <c r="G98" s="176"/>
-      <c r="H98" s="176"/>
-    </row>
-    <row r="99" spans="6:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F99" s="176"/>
-      <c r="G99" s="176"/>
-      <c r="H99" s="176"/>
-    </row>
-    <row r="100" spans="6:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F100" s="176"/>
-      <c r="G100" s="176"/>
-      <c r="H100" s="176"/>
-    </row>
-    <row r="101" spans="6:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F101" s="176"/>
-      <c r="G101" s="176"/>
-      <c r="H101" s="176"/>
+    <row r="54" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F54" s="139"/>
+      <c r="G54" s="139"/>
+      <c r="H54" s="139"/>
+    </row>
+    <row r="55" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F55" s="139"/>
+      <c r="G55" s="139"/>
+      <c r="H55" s="139"/>
+    </row>
+    <row r="56" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F56" s="139"/>
+      <c r="G56" s="139"/>
+      <c r="H56" s="139"/>
+    </row>
+    <row r="57" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F57" s="139"/>
+      <c r="G57" s="139"/>
+      <c r="H57" s="139"/>
+    </row>
+    <row r="58" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F58" s="139"/>
+      <c r="G58" s="139"/>
+      <c r="H58" s="139"/>
+    </row>
+    <row r="59" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F59" s="139"/>
+      <c r="G59" s="139"/>
+      <c r="H59" s="139"/>
+    </row>
+    <row r="60" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F60" s="139"/>
+      <c r="G60" s="139"/>
+      <c r="H60" s="139"/>
+    </row>
+    <row r="61" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F61" s="139"/>
+      <c r="G61" s="139"/>
+      <c r="H61" s="139"/>
+    </row>
+    <row r="62" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F62" s="139"/>
+      <c r="G62" s="139"/>
+      <c r="H62" s="139"/>
+    </row>
+    <row r="63" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F63" s="139"/>
+      <c r="G63" s="139"/>
+      <c r="H63" s="139"/>
+    </row>
+    <row r="64" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F64" s="139"/>
+      <c r="G64" s="139"/>
+      <c r="H64" s="139"/>
+    </row>
+    <row r="65" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F65" s="139"/>
+      <c r="G65" s="139"/>
+      <c r="H65" s="139"/>
+    </row>
+    <row r="66" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F66" s="139"/>
+      <c r="G66" s="139"/>
+      <c r="H66" s="139"/>
+    </row>
+    <row r="67" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F67" s="139"/>
+      <c r="G67" s="139"/>
+      <c r="H67" s="139"/>
+    </row>
+    <row r="68" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F68" s="139"/>
+      <c r="G68" s="139"/>
+      <c r="H68" s="139"/>
+    </row>
+    <row r="69" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F69" s="139"/>
+      <c r="G69" s="139"/>
+      <c r="H69" s="139"/>
+    </row>
+    <row r="70" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F70" s="139"/>
+      <c r="G70" s="139"/>
+      <c r="H70" s="139"/>
+    </row>
+    <row r="71" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F71" s="139"/>
+      <c r="G71" s="139"/>
+      <c r="H71" s="139"/>
+    </row>
+    <row r="72" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F72" s="139"/>
+      <c r="G72" s="139"/>
+      <c r="H72" s="139"/>
+    </row>
+    <row r="73" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F73" s="139"/>
+      <c r="G73" s="139"/>
+      <c r="H73" s="139"/>
+    </row>
+    <row r="74" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F74" s="139"/>
+      <c r="G74" s="139"/>
+      <c r="H74" s="139"/>
+    </row>
+    <row r="75" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F75" s="139"/>
+      <c r="G75" s="139"/>
+      <c r="H75" s="139"/>
+    </row>
+    <row r="76" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F76" s="139"/>
+      <c r="G76" s="139"/>
+      <c r="H76" s="139"/>
+      <c r="S76" s="70"/>
+    </row>
+    <row r="77" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F77" s="139"/>
+      <c r="G77" s="139"/>
+      <c r="H77" s="139"/>
+    </row>
+    <row r="78" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F78" s="139"/>
+      <c r="G78" s="139"/>
+      <c r="H78" s="139"/>
+    </row>
+    <row r="79" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F79" s="139"/>
+      <c r="G79" s="139"/>
+      <c r="H79" s="139"/>
+    </row>
+    <row r="80" spans="6:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F80" s="139"/>
+      <c r="G80" s="139"/>
+      <c r="H80" s="139"/>
+    </row>
+    <row r="81" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F81" s="139"/>
+      <c r="G81" s="139"/>
+      <c r="H81" s="139"/>
+    </row>
+    <row r="82" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F82" s="139"/>
+      <c r="G82" s="139"/>
+      <c r="H82" s="139"/>
+    </row>
+    <row r="83" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F83" s="139"/>
+      <c r="G83" s="139"/>
+      <c r="H83" s="139"/>
+      <c r="Q83" s="156"/>
+    </row>
+    <row r="84" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F84" s="139"/>
+      <c r="G84" s="139"/>
+      <c r="H84" s="139"/>
+    </row>
+    <row r="85" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F85" s="139"/>
+      <c r="G85" s="139"/>
+      <c r="H85" s="139"/>
+    </row>
+    <row r="86" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F86" s="139"/>
+      <c r="G86" s="139"/>
+      <c r="H86" s="139"/>
+    </row>
+    <row r="87" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F87" s="139"/>
+      <c r="G87" s="139"/>
+      <c r="H87" s="139"/>
+    </row>
+    <row r="88" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F88" s="139"/>
+      <c r="G88" s="139"/>
+      <c r="H88" s="139"/>
+    </row>
+    <row r="89" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F89" s="139"/>
+      <c r="G89" s="139"/>
+      <c r="H89" s="139"/>
+    </row>
+    <row r="90" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F90" s="139"/>
+      <c r="G90" s="139"/>
+      <c r="H90" s="139"/>
+    </row>
+    <row r="91" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F91" s="139"/>
+      <c r="G91" s="139"/>
+      <c r="H91" s="139"/>
+    </row>
+    <row r="92" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F92" s="139"/>
+      <c r="G92" s="139"/>
+      <c r="H92" s="139"/>
+    </row>
+    <row r="93" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F93" s="139"/>
+      <c r="G93" s="139"/>
+      <c r="H93" s="139"/>
+    </row>
+    <row r="94" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F94" s="139"/>
+      <c r="G94" s="139"/>
+      <c r="H94" s="139"/>
+    </row>
+    <row r="95" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F95" s="139"/>
+      <c r="G95" s="139"/>
+      <c r="H95" s="139"/>
+    </row>
+    <row r="96" spans="6:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F96" s="139"/>
+      <c r="G96" s="139"/>
+      <c r="H96" s="139"/>
+    </row>
+    <row r="97" spans="6:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F97" s="139"/>
+      <c r="G97" s="139"/>
+      <c r="H97" s="139"/>
+    </row>
+    <row r="98" spans="6:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F98" s="139"/>
+      <c r="G98" s="139"/>
+      <c r="H98" s="139"/>
+    </row>
+    <row r="99" spans="6:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F99" s="139"/>
+      <c r="G99" s="139"/>
+      <c r="H99" s="139"/>
+    </row>
+    <row r="100" spans="6:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F100" s="139"/>
+      <c r="G100" s="139"/>
+      <c r="H100" s="139"/>
+    </row>
+    <row r="101" spans="6:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F101" s="139"/>
+      <c r="G101" s="139"/>
+      <c r="H101" s="139"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="K10:N10"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="K15:N15"/>
     <mergeCell ref="P18:S18"/>
@@ -4388,18 +4398,11 @@
     <mergeCell ref="K22:M22"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G11" xr:uid="{8B73DCD5-E3A9-4DCE-8476-C0A45F451077}">
@@ -4421,32 +4424,32 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40" style="24" customWidth="1"/>
-    <col min="4" max="6" width="13.7109375" style="2" customWidth="1"/>
-    <col min="7" max="11" width="13.7109375" style="1" customWidth="1"/>
-    <col min="12" max="21" width="15.7109375" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="13.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40" style="23" customWidth="1"/>
+    <col min="4" max="6" width="13.6640625" style="2" customWidth="1"/>
+    <col min="7" max="11" width="13.6640625" style="1" customWidth="1"/>
+    <col min="12" max="21" width="15.6640625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+    <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="198" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="198"/>
+      <c r="C5" s="198"/>
+      <c r="D5" s="198"/>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
     </row>
-    <row r="6" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
@@ -4455,7 +4458,7 @@
       <c r="J6"/>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
@@ -4467,7 +4470,7 @@
       <c r="J7"/>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="21" t="s">
         <v>39</v>
       </c>
@@ -4483,7 +4486,7 @@
       <c r="J8"/>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
         <v>38</v>
       </c>
@@ -4499,7 +4502,7 @@
       <c r="J9"/>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
         <v>36</v>
       </c>
@@ -4515,11 +4518,11 @@
       <c r="J10"/>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="24">
         <f>C12/C10</f>
         <v>0.64038811400848994</v>
       </c>
@@ -4532,7 +4535,7 @@
       <c r="J11"/>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="13" t="s">
         <v>34</v>
       </c>
@@ -4549,7 +4552,7 @@
       <c r="J12"/>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="13" t="s">
         <v>33</v>
       </c>
@@ -4565,7 +4568,7 @@
       <c r="J13"/>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="13" t="s">
         <v>32</v>
       </c>
@@ -4581,7 +4584,7 @@
       <c r="J14"/>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="13" t="s">
         <v>31</v>
       </c>
@@ -4598,7 +4601,7 @@
       <c r="J15"/>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="13" t="s">
         <v>30</v>
       </c>
@@ -4614,7 +4617,7 @@
       <c r="J16"/>
       <c r="K16"/>
     </row>
-    <row r="17" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="13" t="s">
         <v>29</v>
       </c>
@@ -4630,7 +4633,7 @@
       <c r="J17"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="13" t="s">
         <v>28</v>
       </c>
@@ -4641,7 +4644,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="13" t="s">
         <v>27</v>
       </c>
@@ -4653,7 +4656,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="13" t="s">
         <v>26</v>
       </c>
@@ -4665,7 +4668,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="13" t="s">
         <v>24</v>
       </c>
@@ -4675,11 +4678,11 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="25">
         <v>0.76600000000000001</v>
       </c>
       <c r="D22"/>
@@ -4687,11 +4690,11 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="25">
         <v>0.48799999999999999</v>
       </c>
       <c r="D23"/>
@@ -4699,11 +4702,11 @@
       <c r="F23" s="1"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="27">
+      <c r="C24" s="26">
         <f>C23/C22</f>
         <v>0.63707571801566576</v>
       </c>
@@ -4711,30 +4714,30 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="2:13" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="28"/>
+      <c r="C25" s="27"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="2:13" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="28"/>
+      <c r="C26" s="27"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="28"/>
+      <c r="C27" s="27"/>
       <c r="D27"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="13" t="s">
         <v>16</v>
       </c>
@@ -4752,7 +4755,7 @@
       <c r="L28" s="14"/>
       <c r="M28" s="14"/>
     </row>
-    <row r="29" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="13" t="s">
         <v>15</v>
       </c>
@@ -4770,7 +4773,7 @@
       <c r="L29" s="14"/>
       <c r="M29" s="14"/>
     </row>
-    <row r="30" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="13" t="s">
         <v>14</v>
       </c>
@@ -4788,7 +4791,7 @@
       <c r="L30" s="14"/>
       <c r="M30" s="14"/>
     </row>
-    <row r="31" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="15" t="s">
         <v>13</v>
       </c>
@@ -4807,7 +4810,7 @@
       <c r="L31" s="14"/>
       <c r="M31" s="14"/>
     </row>
-    <row r="32" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="15" t="s">
         <v>12</v>
       </c>
@@ -4826,7 +4829,7 @@
       <c r="L32" s="14"/>
       <c r="M32" s="14"/>
     </row>
-    <row r="33" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="13" t="s">
         <v>11</v>
       </c>
@@ -4838,7 +4841,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="11" t="s">
         <v>10</v>
       </c>
@@ -4847,7 +4850,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35"/>
       <c r="C35" s="6"/>
       <c r="J35" s="9"/>
@@ -4860,7 +4863,7 @@
       <c r="Q35" s="9"/>
       <c r="R35" s="9"/>
     </row>
-    <row r="36" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="6"/>
       <c r="D36"/>
       <c r="E36"/>
@@ -4878,7 +4881,7 @@
       <c r="Q36" s="9"/>
       <c r="R36" s="9"/>
     </row>
-    <row r="37" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37"/>
       <c r="B37" s="4" t="s">
         <v>9</v>
@@ -4902,7 +4905,7 @@
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
     </row>
-    <row r="38" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38"/>
       <c r="B38" s="4" t="s">
         <v>8</v>
@@ -4926,7 +4929,7 @@
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
     </row>
-    <row r="39" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39"/>
       <c r="B39" s="4" t="s">
         <v>7</v>
@@ -4950,7 +4953,7 @@
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
     </row>
-    <row r="40" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40"/>
       <c r="B40" s="4" t="s">
         <v>6</v>
@@ -4974,7 +4977,7 @@
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
     </row>
-    <row r="41" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A41"/>
       <c r="B41" s="7"/>
       <c r="C41" s="6"/>
@@ -4987,7 +4990,7 @@
       <c r="J41"/>
       <c r="K41"/>
     </row>
-    <row r="42" spans="1:18" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42"/>
       <c r="B42" s="4" t="s">
         <v>5</v>
@@ -5005,7 +5008,7 @@
       <c r="J42"/>
       <c r="K42"/>
     </row>
-    <row r="43" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A43"/>
       <c r="B43" s="4" t="s">
         <v>4</v>
@@ -5023,7 +5026,7 @@
       <c r="J43"/>
       <c r="K43"/>
     </row>
-    <row r="44" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A44"/>
       <c r="B44" s="7"/>
       <c r="C44" s="6"/>
@@ -5036,7 +5039,7 @@
       <c r="J44"/>
       <c r="K44"/>
     </row>
-    <row r="45" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A45"/>
       <c r="B45" s="4" t="s">
         <v>3</v>
@@ -5054,7 +5057,7 @@
       <c r="J45"/>
       <c r="K45"/>
     </row>
-    <row r="46" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A46"/>
       <c r="B46" s="4" t="s">
         <v>2</v>
@@ -5074,7 +5077,7 @@
       <c r="J46"/>
       <c r="K46"/>
     </row>
-    <row r="47" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A47"/>
       <c r="B47" s="4" t="s">
         <v>0</v>
@@ -5095,7 +5098,7 @@
       <c r="J47"/>
       <c r="K47"/>
     </row>
-    <row r="48" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48" s="6"/>
@@ -5108,7 +5111,7 @@
       <c r="J48"/>
       <c r="K48"/>
     </row>
-    <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49" s="6"/>
@@ -5121,7 +5124,7 @@
       <c r="J49"/>
       <c r="K49"/>
     </row>
-    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50" s="6"/>
@@ -5134,7 +5137,7 @@
       <c r="J50"/>
       <c r="K50"/>
     </row>
-    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51" s="6"/>
@@ -5147,7 +5150,7 @@
       <c r="J51"/>
       <c r="K51"/>
     </row>
-    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52" s="6"/>
@@ -5160,7 +5163,7 @@
       <c r="J52"/>
       <c r="K52"/>
     </row>
-    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53" s="6"/>
@@ -5173,7 +5176,7 @@
       <c r="J53"/>
       <c r="K53"/>
     </row>
-    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54" s="6"/>
@@ -5186,7 +5189,7 @@
       <c r="J54"/>
       <c r="K54"/>
     </row>
-    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55" s="6"/>
@@ -5199,7 +5202,7 @@
       <c r="J55"/>
       <c r="K55"/>
     </row>
-    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56" s="6"/>
@@ -5212,7 +5215,7 @@
       <c r="J56"/>
       <c r="K56"/>
     </row>
-    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57" s="6"/>
@@ -5225,7 +5228,7 @@
       <c r="J57"/>
       <c r="K57"/>
     </row>
-    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58" s="6"/>
@@ -5238,7 +5241,7 @@
       <c r="J58"/>
       <c r="K58"/>
     </row>
-    <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59" s="6"/>
@@ -5251,7 +5254,7 @@
       <c r="J59"/>
       <c r="K59"/>
     </row>
-    <row r="60" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60" s="6"/>
@@ -5264,7 +5267,7 @@
       <c r="J60"/>
       <c r="K60"/>
     </row>
-    <row r="61" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61" s="6"/>
@@ -5277,7 +5280,7 @@
       <c r="J61"/>
       <c r="K61"/>
     </row>
-    <row r="62" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62" s="6"/>
@@ -5290,7 +5293,7 @@
       <c r="J62"/>
       <c r="K62"/>
     </row>
-    <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63" s="6"/>
@@ -5303,7 +5306,7 @@
       <c r="J63"/>
       <c r="K63"/>
     </row>
-    <row r="64" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64" s="6"/>
@@ -5316,7 +5319,7 @@
       <c r="J64"/>
       <c r="K64"/>
     </row>
-    <row r="65" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65" s="6"/>
@@ -5329,7 +5332,7 @@
       <c r="J65"/>
       <c r="K65"/>
     </row>
-    <row r="66" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66" s="6"/>
@@ -5342,7 +5345,7 @@
       <c r="J66"/>
       <c r="K66"/>
     </row>
-    <row r="67" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67" s="6"/>
@@ -5355,7 +5358,7 @@
       <c r="J67"/>
       <c r="K67"/>
     </row>
-    <row r="68" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68" s="6"/>
@@ -5368,7 +5371,7 @@
       <c r="J68"/>
       <c r="K68"/>
     </row>
-    <row r="69" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69" s="6"/>
@@ -5381,7 +5384,7 @@
       <c r="J69"/>
       <c r="K69"/>
     </row>
-    <row r="70" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70" s="6"/>
@@ -5394,7 +5397,7 @@
       <c r="J70"/>
       <c r="K70"/>
     </row>
-    <row r="71" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71" s="6"/>
@@ -5407,7 +5410,7 @@
       <c r="J71"/>
       <c r="K71"/>
     </row>
-    <row r="72" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72" s="6"/>
@@ -5420,7 +5423,7 @@
       <c r="J72"/>
       <c r="K72"/>
     </row>
-    <row r="73" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73" s="6"/>
@@ -5433,7 +5436,7 @@
       <c r="J73"/>
       <c r="K73"/>
     </row>
-    <row r="74" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74" s="6"/>
@@ -5446,7 +5449,7 @@
       <c r="J74"/>
       <c r="K74"/>
     </row>
-    <row r="75" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75" s="6"/>
@@ -5459,7 +5462,7 @@
       <c r="J75"/>
       <c r="K75"/>
     </row>
-    <row r="76" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76" s="6"/>
@@ -5472,7 +5475,7 @@
       <c r="J76"/>
       <c r="K76"/>
     </row>
-    <row r="77" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77" s="6"/>
@@ -5485,7 +5488,7 @@
       <c r="J77"/>
       <c r="K77"/>
     </row>
-    <row r="78" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78" s="6"/>
@@ -5498,7 +5501,7 @@
       <c r="J78"/>
       <c r="K78"/>
     </row>
-    <row r="79" spans="1:37" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:37" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79" s="6"/>
@@ -5537,7 +5540,7 @@
       <c r="AJ79" s="1"/>
       <c r="AK79" s="1"/>
     </row>
-    <row r="80" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:37" ht="15" x14ac:dyDescent="0.2">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80" s="6"/>
@@ -5550,7 +5553,7 @@
       <c r="J80"/>
       <c r="K80"/>
     </row>
-    <row r="81" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81" s="6"/>
@@ -5563,7 +5566,7 @@
       <c r="J81"/>
       <c r="K81"/>
     </row>
-    <row r="82" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82" s="6"/>
@@ -5576,7 +5579,7 @@
       <c r="J82"/>
       <c r="K82"/>
     </row>
-    <row r="83" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83" s="6"/>
@@ -5589,7 +5592,7 @@
       <c r="J83"/>
       <c r="K83"/>
     </row>
-    <row r="84" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84" s="6"/>
@@ -5602,7 +5605,7 @@
       <c r="J84"/>
       <c r="K84"/>
     </row>
-    <row r="85" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85" s="6"/>
@@ -5615,7 +5618,7 @@
       <c r="J85"/>
       <c r="K85"/>
     </row>
-    <row r="86" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86" s="6"/>
@@ -5628,23 +5631,23 @@
       <c r="J86"/>
       <c r="K86"/>
     </row>
-    <row r="87" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="B87"/>
       <c r="C87" s="6"/>
     </row>
-    <row r="88" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="B88"/>
       <c r="C88" s="6"/>
     </row>
-    <row r="89" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="B89"/>
       <c r="C89" s="6"/>
     </row>
-    <row r="90" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="B90"/>
       <c r="C90" s="6"/>
     </row>
-    <row r="91" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="B91"/>
       <c r="C91" s="6"/>
     </row>

</xml_diff>